<commit_message>
Added format to dashboard
</commit_message>
<xml_diff>
--- a/data/processed/diccionario_datos_iter_00CSV20_modified.xlsx
+++ b/data/processed/diccionario_datos_iter_00CSV20_modified.xlsx
@@ -3253,16 +3253,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3273,6 +3264,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3594,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B166" sqref="B166"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Removed data that was not used
</commit_message>
<xml_diff>
--- a/data/processed/diccionario_datos_iter_00CSV20_modified.xlsx
+++ b/data/processed/diccionario_datos_iter_00CSV20_modified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://winliveudlap-my.sharepoint.com/personal/marco_bravoml_udlap_mx/Documents/Documents/MDS/Block 6/DSCI 532/DSCI_532_individual-assignment_marcony1/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{0718C61D-7051-43B4-B282-1FB5599B1572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D18DB27E-3226-41DF-8679-8D46D89EBA1D}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{0718C61D-7051-43B4-B282-1FB5599B1572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AEFA38C-F553-4E3A-9FC4-A37C73142C69}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3589,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>41</v>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
@@ -3894,7 +3894,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
@@ -3917,7 +3917,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
@@ -3940,7 +3940,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>55</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>65</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>68</v>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
@@ -4101,7 +4101,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>80</v>
@@ -4147,7 +4147,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>83</v>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>86</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>92</v>
@@ -4239,7 +4239,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>98</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
         <v>101</v>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>104</v>
@@ -4331,7 +4331,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>107</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
         <v>110</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>113</v>
@@ -4400,7 +4400,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>116</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>119</v>
@@ -4446,7 +4446,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>122</v>
@@ -4469,7 +4469,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
         <v>125</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
         <v>128</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
         <v>131</v>
@@ -4538,7 +4538,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
         <v>134</v>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>137</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>140</v>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>143</v>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
         <v>146</v>
@@ -4653,7 +4653,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>149</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>152</v>
@@ -4699,7 +4699,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
         <v>155</v>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
         <v>158</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
         <v>161</v>
@@ -4768,7 +4768,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
         <v>164</v>
@@ -4791,7 +4791,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
         <v>167</v>
@@ -4814,7 +4814,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
         <v>170</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>173</v>
@@ -4860,7 +4860,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>176</v>
@@ -4883,7 +4883,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>179</v>
@@ -4906,7 +4906,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>182</v>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>185</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>188</v>
@@ -4975,7 +4975,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>191</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>194</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>197</v>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>200</v>
@@ -5067,7 +5067,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>203</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>206</v>
@@ -5113,7 +5113,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>209</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>212</v>
@@ -5159,7 +5159,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>215</v>
@@ -5182,7 +5182,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>218</v>
@@ -5205,7 +5205,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>221</v>
@@ -5228,7 +5228,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>224</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>227</v>
@@ -5274,7 +5274,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>230</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>233</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>236</v>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>239</v>
@@ -5366,7 +5366,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>242</v>
@@ -5389,7 +5389,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>245</v>
@@ -5412,7 +5412,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>248</v>
@@ -5435,7 +5435,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>251</v>
@@ -5458,7 +5458,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>254</v>
@@ -5481,7 +5481,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>257</v>
@@ -5504,7 +5504,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>260</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>263</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>266</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>269</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>272</v>
@@ -5619,7 +5619,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>275</v>
@@ -5642,7 +5642,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>278</v>
@@ -5665,7 +5665,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>281</v>
@@ -5688,7 +5688,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>284</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>287</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>290</v>
@@ -5757,7 +5757,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>293</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>296</v>
@@ -5803,7 +5803,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>299</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>302</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>305</v>
@@ -5872,7 +5872,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>308</v>
@@ -5895,7 +5895,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>311</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>314</v>
@@ -5941,7 +5941,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>317</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>320</v>
@@ -5987,7 +5987,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>323</v>
@@ -6010,7 +6010,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>326</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>329</v>
@@ -6056,7 +6056,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>332</v>
@@ -6079,7 +6079,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>335</v>
@@ -6102,7 +6102,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>338</v>
@@ -6125,7 +6125,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>341</v>
@@ -6148,7 +6148,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>344</v>
@@ -6171,7 +6171,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>347</v>
@@ -6194,7 +6194,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>350</v>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>353</v>
@@ -6240,7 +6240,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>356</v>
@@ -6263,7 +6263,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>359</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>362</v>
@@ -6309,7 +6309,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>365</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>368</v>
@@ -6355,7 +6355,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>371</v>
@@ -6378,7 +6378,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>374</v>
@@ -6401,7 +6401,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>377</v>
@@ -6424,7 +6424,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>380</v>
@@ -6447,7 +6447,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>383</v>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>386</v>
@@ -6493,7 +6493,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>389</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>392</v>
@@ -6539,7 +6539,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>395</v>
@@ -6562,7 +6562,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>398</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>401</v>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>404</v>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>407</v>
@@ -6654,7 +6654,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>410</v>
@@ -6677,7 +6677,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B138" t="s">
         <v>413</v>
@@ -6700,7 +6700,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B139" t="s">
         <v>416</v>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="B140" t="s">
         <v>419</v>
@@ -6746,7 +6746,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>422</v>
@@ -6769,7 +6769,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>425</v>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>428</v>
@@ -6815,7 +6815,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>431</v>
@@ -6838,7 +6838,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>434</v>
@@ -6861,7 +6861,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B146" t="s">
         <v>437</v>
@@ -6884,7 +6884,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B147" t="s">
         <v>440</v>
@@ -6907,7 +6907,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B148" t="s">
         <v>443</v>
@@ -6930,7 +6930,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B149" t="s">
         <v>446</v>
@@ -6953,7 +6953,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B150" t="s">
         <v>449</v>
@@ -6976,7 +6976,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B151" t="s">
         <v>452</v>
@@ -6999,7 +6999,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>455</v>
@@ -7022,7 +7022,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B153" t="s">
         <v>458</v>
@@ -7045,7 +7045,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B154" t="s">
         <v>461</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B155" t="s">
         <v>464</v>
@@ -7091,7 +7091,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B156" t="s">
         <v>467</v>
@@ -7114,7 +7114,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B157" t="s">
         <v>470</v>
@@ -7137,7 +7137,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B158" t="s">
         <v>473</v>
@@ -7160,7 +7160,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B159" t="s">
         <v>476</v>
@@ -7183,7 +7183,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>479</v>
@@ -7206,7 +7206,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>482</v>
@@ -7229,7 +7229,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>485</v>
@@ -7252,7 +7252,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>488</v>
@@ -7275,7 +7275,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>491</v>
@@ -7298,7 +7298,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>494</v>
@@ -7321,7 +7321,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>497</v>
@@ -7344,7 +7344,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B167" s="6" t="s">
         <v>500</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B168" s="6" t="s">
         <v>503</v>
@@ -7390,7 +7390,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B169" s="6" t="s">
         <v>506</v>
@@ -7413,7 +7413,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>509</v>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>512</v>
@@ -7459,7 +7459,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>515</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>518</v>
@@ -7505,7 +7505,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B174" s="6" t="s">
         <v>521</v>
@@ -7528,7 +7528,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>524</v>
@@ -7551,7 +7551,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>527</v>
@@ -7574,7 +7574,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>530</v>
@@ -7597,7 +7597,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>533</v>
@@ -7620,7 +7620,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>536</v>
@@ -7643,7 +7643,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>539</v>
@@ -7666,7 +7666,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>542</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>545</v>
@@ -7712,7 +7712,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>548</v>
@@ -7735,7 +7735,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>551</v>
@@ -7758,7 +7758,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>554</v>
@@ -7781,7 +7781,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>557</v>
@@ -7804,7 +7804,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>560</v>
@@ -7827,7 +7827,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B188" s="6" t="s">
         <v>563</v>
@@ -7850,7 +7850,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B189" s="6" t="s">
         <v>566</v>
@@ -7873,7 +7873,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="B190" s="6" t="s">
         <v>569</v>
@@ -7896,7 +7896,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B191" s="6" t="s">
         <v>572</v>
@@ -7919,7 +7919,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>575</v>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A193">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>578</v>
@@ -7965,7 +7965,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A194">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>581</v>
@@ -7988,7 +7988,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A195">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>584</v>
@@ -8011,7 +8011,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A196">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B196" s="6" t="s">
         <v>587</v>
@@ -8034,7 +8034,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A197">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>590</v>
@@ -8057,7 +8057,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A198">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>593</v>
@@ -8080,7 +8080,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A199">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B199" s="6" t="s">
         <v>596</v>
@@ -8103,7 +8103,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A200">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="B200" s="6" t="s">
         <v>599</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A201">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>602</v>
@@ -8149,7 +8149,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A202">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>605</v>
@@ -8172,7 +8172,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A203">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B203" s="7" t="s">
         <v>608</v>
@@ -8195,7 +8195,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A204">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B204" s="7" t="s">
         <v>612</v>
@@ -8218,7 +8218,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A205">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B205" s="7" t="s">
         <v>615</v>
@@ -8241,7 +8241,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A206">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B206" s="7" t="s">
         <v>618</v>
@@ -8264,7 +8264,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A207">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B207" s="7" t="s">
         <v>621</v>
@@ -8287,7 +8287,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A208">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="B208" s="7" t="s">
         <v>624</v>
@@ -8310,7 +8310,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A209">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B209" s="7" t="s">
         <v>627</v>
@@ -8333,7 +8333,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A210">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B210" s="7" t="s">
         <v>630</v>
@@ -8356,7 +8356,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A211">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B211" s="7" t="s">
         <v>633</v>
@@ -8379,7 +8379,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A212">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B212" s="7" t="s">
         <v>636</v>
@@ -8402,7 +8402,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A213">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B213" s="7" t="s">
         <v>639</v>
@@ -8425,7 +8425,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A214">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B214" s="7" t="s">
         <v>642</v>
@@ -8448,7 +8448,7 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A215">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B215" s="8" t="s">
         <v>645</v>
@@ -8471,7 +8471,7 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A216">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>648</v>
@@ -8494,7 +8494,7 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A217">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B217" t="s">
         <v>651</v>
@@ -8517,7 +8517,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A218">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B218" t="s">
         <v>654</v>
@@ -8540,7 +8540,7 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A219">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="B219" t="s">
         <v>657</v>
@@ -8563,7 +8563,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A220">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B220" t="s">
         <v>660</v>
@@ -8586,7 +8586,7 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A221">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B221" t="s">
         <v>663</v>
@@ -8609,7 +8609,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A222">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B222" t="s">
         <v>666</v>
@@ -8632,7 +8632,7 @@
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A223">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B223" t="s">
         <v>669</v>
@@ -8655,7 +8655,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A224">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="B224" t="s">
         <v>672</v>
@@ -8678,7 +8678,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A225">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B225" s="9" t="s">
         <v>675</v>
@@ -8701,7 +8701,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A226">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B226" s="9" t="s">
         <v>678</v>
@@ -8724,7 +8724,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A227">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B227" s="9" t="s">
         <v>681</v>
@@ -8747,7 +8747,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A228">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B228" s="7" t="s">
         <v>684</v>
@@ -8770,7 +8770,7 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A229">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B229" s="7" t="s">
         <v>687</v>
@@ -8793,7 +8793,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A230">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B230" s="7" t="s">
         <v>690</v>
@@ -8816,7 +8816,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A231">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B231" s="7" t="s">
         <v>693</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A232">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>696</v>
@@ -8862,7 +8862,7 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A233">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>699</v>
@@ -8885,7 +8885,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A234">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>702</v>
@@ -8908,7 +8908,7 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A235">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>705</v>
@@ -8931,7 +8931,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A236">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>709</v>
@@ -8954,7 +8954,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A237">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>712</v>
@@ -8977,7 +8977,7 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A238">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="B238" t="s">
         <v>715</v>
@@ -9000,7 +9000,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A239">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="B239" t="s">
         <v>718</v>
@@ -9023,7 +9023,7 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A240">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B240" t="s">
         <v>721</v>
@@ -9046,7 +9046,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A241">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="B241" t="s">
         <v>724</v>
@@ -9069,7 +9069,7 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A242">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B242" t="s">
         <v>727</v>
@@ -9092,7 +9092,7 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A243">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B243" t="s">
         <v>730</v>
@@ -9115,7 +9115,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A244">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="B244" t="s">
         <v>733</v>
@@ -9138,7 +9138,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A245">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="B245" t="s">
         <v>736</v>
@@ -9161,7 +9161,7 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A246">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="B246" t="s">
         <v>739</v>
@@ -9184,7 +9184,7 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A247">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B247" t="s">
         <v>742</v>
@@ -9207,7 +9207,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A248">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B248" t="s">
         <v>745</v>
@@ -9230,7 +9230,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A249">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B249" t="s">
         <v>748</v>
@@ -9253,7 +9253,7 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A250">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="B250" t="s">
         <v>751</v>
@@ -9276,7 +9276,7 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A251">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B251" t="s">
         <v>754</v>
@@ -9299,7 +9299,7 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A252">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B252" t="s">
         <v>758</v>
@@ -9322,7 +9322,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A253">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B253" t="s">
         <v>761</v>
@@ -9345,7 +9345,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A254">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B254" t="s">
         <v>764</v>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A255">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B255" t="s">
         <v>767</v>
@@ -9391,7 +9391,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A256">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B256" t="s">
         <v>770</v>
@@ -9414,7 +9414,7 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A257">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B257" t="s">
         <v>773</v>
@@ -9437,7 +9437,7 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A258">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B258" t="s">
         <v>776</v>
@@ -9460,7 +9460,7 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A259">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="B259" t="s">
         <v>779</v>
@@ -9483,7 +9483,7 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A260">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="B260" t="s">
         <v>782</v>
@@ -9506,7 +9506,7 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A261">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="B261" t="s">
         <v>785</v>
@@ -9529,7 +9529,7 @@
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A262">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="B262" t="s">
         <v>788</v>
@@ -9552,7 +9552,7 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A263">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B263" t="s">
         <v>791</v>
@@ -9575,7 +9575,7 @@
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A264">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B264" t="s">
         <v>794</v>
@@ -9598,7 +9598,7 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A265">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="B265" t="s">
         <v>797</v>
@@ -9621,7 +9621,7 @@
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A266">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="B266" t="s">
         <v>800</v>
@@ -9644,7 +9644,7 @@
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A267">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="B267" t="s">
         <v>803</v>
@@ -9667,7 +9667,7 @@
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A268">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="B268" t="s">
         <v>806</v>
@@ -9690,7 +9690,7 @@
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A269">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B269" t="s">
         <v>809</v>
@@ -9713,7 +9713,7 @@
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A270">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="B270" t="s">
         <v>812</v>
@@ -9736,7 +9736,7 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A271">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="B271" t="s">
         <v>815</v>
@@ -9759,7 +9759,7 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A272">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B272" t="s">
         <v>818</v>
@@ -9782,7 +9782,7 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A273">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B273" t="s">
         <v>821</v>
@@ -9805,7 +9805,7 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A274">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B274" t="s">
         <v>824</v>
@@ -9828,7 +9828,7 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A275">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="B275" t="s">
         <v>827</v>
@@ -9851,7 +9851,7 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A276">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="B276" t="s">
         <v>830</v>
@@ -9874,7 +9874,7 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A277">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B277" t="s">
         <v>833</v>
@@ -9897,7 +9897,7 @@
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A278">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B278" t="s">
         <v>836</v>
@@ -9920,7 +9920,7 @@
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A279">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B279" t="s">
         <v>839</v>
@@ -9943,7 +9943,7 @@
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A280">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B280" t="s">
         <v>842</v>
@@ -9966,7 +9966,7 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A281">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="B281" t="s">
         <v>845</v>
@@ -9989,7 +9989,7 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A282">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="B282" t="s">
         <v>848</v>
@@ -10012,7 +10012,7 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A283">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="B283" t="s">
         <v>851</v>
@@ -10035,7 +10035,7 @@
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A284">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B284" t="s">
         <v>854</v>
@@ -10058,7 +10058,7 @@
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A285">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="B285" t="s">
         <v>857</v>
@@ -10081,7 +10081,7 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A286">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B286" t="s">
         <v>860</v>
@@ -10104,7 +10104,7 @@
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A287">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="B287" t="s">
         <v>863</v>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A288">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B288" t="s">
         <v>866</v>
@@ -10150,7 +10150,7 @@
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A289">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B289" t="s">
         <v>869</v>
@@ -10173,7 +10173,7 @@
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A290">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B290" t="s">
         <v>872</v>
@@ -10196,7 +10196,7 @@
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A291">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="B291" t="s">
         <v>875</v>

</xml_diff>